<commit_message>
Attempt to add metadata, summarized EMLAB units
</commit_message>
<xml_diff>
--- a/resources/configurations/COMPETES EU 2050-KIP config.xlsx
+++ b/resources/configurations/COMPETES EU 2050-KIP config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\workspace\Spine_EMLab_COMPETES\resources\configurations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3D99017-D8EA-485C-AB26-C8EE103B7E81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BD38B32-8D10-4C1A-AD0D-2CB587015204}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="480" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4590" yWindow="5190" windowWidth="28800" windowHeight="15435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Object Type 1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="88">
   <si>
     <t>Biomass Potential</t>
   </si>
@@ -218,9 +218,6 @@
   </si>
   <si>
     <t>Line</t>
-  </si>
-  <si>
-    <t>InvCountry</t>
   </si>
   <si>
     <t>TechnOrder</t>
@@ -618,7 +615,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
@@ -709,8 +706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3C637E7-CEF7-493D-BBA4-CB3536D77CE6}">
   <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -943,7 +940,7 @@
         <v>30</v>
       </c>
       <c r="C21" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -987,7 +984,7 @@
         <v>30</v>
       </c>
       <c r="C25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -998,7 +995,7 @@
         <v>50</v>
       </c>
       <c r="C26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -1009,7 +1006,7 @@
         <v>51</v>
       </c>
       <c r="C27" t="s">
-        <v>24</v>
+        <v>56</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -1020,7 +1017,7 @@
         <v>51</v>
       </c>
       <c r="C28" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -1042,7 +1039,7 @@
         <v>24</v>
       </c>
       <c r="C30" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1062,13 +1059,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" t="s">
         <v>72</v>
-      </c>
-      <c r="C1" t="s">
-        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1088,13 +1085,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" t="s">
         <v>72</v>
-      </c>
-      <c r="C1" t="s">
-        <v>73</v>
       </c>
       <c r="D1" t="s">
         <v>32</v>
@@ -1102,27 +1099,27 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" t="s">
         <v>67</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>68</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>69</v>
-      </c>
-      <c r="D2" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3" t="s">
         <v>74</v>
-      </c>
-      <c r="C3" t="s">
-        <v>75</v>
       </c>
       <c r="D3" t="s">
         <v>51</v>
@@ -1153,34 +1150,34 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1211,10 +1208,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C2" t="s">
         <v>56</v>
@@ -1222,10 +1219,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C3" t="s">
         <v>56</v>
@@ -1248,24 +1245,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" t="s">
         <v>72</v>
-      </c>
-      <c r="C1" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" t="s">
         <v>86</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>87</v>
-      </c>
-      <c r="C2" t="s">
-        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1285,13 +1282,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" t="s">
         <v>72</v>
-      </c>
-      <c r="C1" t="s">
-        <v>73</v>
       </c>
       <c r="D1" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
Fixed lost data through imports
</commit_message>
<xml_diff>
--- a/resources/configurations/COMPETES EU 2050-KIP config.xlsx
+++ b/resources/configurations/COMPETES EU 2050-KIP config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\workspace\Spine_EMLab_COMPETES\resources\configurations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BD38B32-8D10-4C1A-AD0D-2CB587015204}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC722BE0-F31D-4342-9A3F-B6826E87736A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4590" yWindow="5190" windowWidth="28800" windowHeight="15435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="480" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Object Type 1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="89">
   <si>
     <t>Biomass Potential</t>
   </si>
@@ -296,6 +296,9 @@
   </si>
   <si>
     <t>Country 2</t>
+  </si>
+  <si>
+    <t>ON-STREAM</t>
   </si>
 </sst>
 </file>
@@ -704,15 +707,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3C637E7-CEF7-493D-BBA4-CB3536D77CE6}">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -723,7 +726,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -734,7 +737,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -745,7 +748,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -756,7 +759,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -767,7 +770,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -778,7 +781,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -789,7 +792,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -800,7 +803,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -811,7 +814,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>34</v>
       </c>
@@ -822,7 +825,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -833,7 +836,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -841,10 +844,13 @@
         <v>24</v>
       </c>
       <c r="C12" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -855,7 +861,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>37</v>
       </c>
@@ -866,7 +872,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>38</v>
       </c>
@@ -877,7 +883,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>39</v>
       </c>
@@ -888,7 +894,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>40</v>
       </c>
@@ -899,7 +905,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>41</v>
       </c>
@@ -910,7 +916,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>42</v>
       </c>
@@ -921,7 +927,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>11</v>
       </c>
@@ -932,7 +938,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>43</v>
       </c>
@@ -943,7 +949,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>44</v>
       </c>
@@ -954,7 +960,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>14</v>
       </c>
@@ -965,7 +971,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>15</v>
       </c>
@@ -976,7 +982,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>16</v>
       </c>
@@ -987,7 +993,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>45</v>
       </c>
@@ -997,8 +1003,11 @@
       <c r="C26" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>18</v>
       </c>
@@ -1008,8 +1017,11 @@
       <c r="C27" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>46</v>
       </c>
@@ -1019,8 +1031,11 @@
       <c r="C28" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>47</v>
       </c>
@@ -1031,7 +1046,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>19</v>
       </c>
@@ -1052,7 +1067,7 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="D56" sqref="D56:D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fixed data lost in mappings, additional type 2 interpretation with multiple indices
</commit_message>
<xml_diff>
--- a/resources/configurations/COMPETES EU 2050-KIP config.xlsx
+++ b/resources/configurations/COMPETES EU 2050-KIP config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\workspace\Spine_EMLab_COMPETES\resources\configurations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC722BE0-F31D-4342-9A3F-B6826E87736A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56F3CA14-6B7A-4587-BF0E-E70F9C40CE2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="480" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="90">
   <si>
     <t>Biomass Potential</t>
   </si>
@@ -299,6 +299,9 @@
   </si>
   <si>
     <t>ON-STREAM</t>
+  </si>
+  <si>
+    <t>InvCountry</t>
   </si>
 </sst>
 </file>
@@ -707,10 +710,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3C637E7-CEF7-493D-BBA4-CB3536D77CE6}">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -894,7 +897,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>40</v>
       </c>
@@ -905,7 +908,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>41</v>
       </c>
@@ -916,7 +919,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>42</v>
       </c>
@@ -927,7 +930,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>11</v>
       </c>
@@ -938,7 +941,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>43</v>
       </c>
@@ -948,8 +951,14 @@
       <c r="C21" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>89</v>
+      </c>
+      <c r="E21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>44</v>
       </c>
@@ -960,7 +969,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>14</v>
       </c>
@@ -971,7 +980,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>15</v>
       </c>
@@ -982,7 +991,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>16</v>
       </c>
@@ -993,7 +1002,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>45</v>
       </c>
@@ -1007,7 +1016,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>18</v>
       </c>
@@ -1021,7 +1030,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>46</v>
       </c>
@@ -1035,7 +1044,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>47</v>
       </c>
@@ -1046,15 +1055,18 @@
         <v>56</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>19</v>
       </c>
       <c r="B30" t="s">
-        <v>24</v>
+        <v>51</v>
       </c>
       <c r="C30" t="s">
         <v>64</v>
+      </c>
+      <c r="D30" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Addition of decentralized generators and changes in import
</commit_message>
<xml_diff>
--- a/resources/configurations/COMPETES EU 2050-KIP config.xlsx
+++ b/resources/configurations/COMPETES EU 2050-KIP config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\workspace\Spine_EMLab_COMPETES\resources\configurations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56F3CA14-6B7A-4587-BF0E-E70F9C40CE2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF236DA9-DCE9-40B9-B67C-2AD0CB2B78A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="480" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="480" windowWidth="38640" windowHeight="21240" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Object Type 1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="91">
   <si>
     <t>Biomass Potential</t>
   </si>
@@ -268,9 +268,6 @@
     <t>NL Installed Capacity (+heat)</t>
   </si>
   <si>
-    <t>NL Installed Capacity-RES (+he</t>
-  </si>
-  <si>
     <t>UNITEU</t>
   </si>
   <si>
@@ -302,6 +299,12 @@
   </si>
   <si>
     <t>InvCountry</t>
+  </si>
+  <si>
+    <t>NL Installed Capacity-RES (+heat)</t>
+  </si>
+  <si>
+    <t>NL Installed Capacity Decentralized (+heat)</t>
   </si>
 </sst>
 </file>
@@ -712,7 +715,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3C637E7-CEF7-493D-BBA4-CB3536D77CE6}">
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
@@ -952,7 +955,7 @@
         <v>56</v>
       </c>
       <c r="D21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E21" t="s">
         <v>26</v>
@@ -1013,7 +1016,7 @@
         <v>63</v>
       </c>
       <c r="D26" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1159,13 +1162,16 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D1116B6-FED4-4FC1-A1F7-3491680046AC}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -1180,7 +1186,7 @@
         <v>75</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1188,7 +1194,7 @@
         <v>76</v>
       </c>
       <c r="B3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1196,15 +1202,23 @@
         <v>77</v>
       </c>
       <c r="B4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="B5" t="s">
-        <v>80</v>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B6" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1235,10 +1249,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C2" t="s">
         <v>56</v>
@@ -1246,10 +1260,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C3" t="s">
         <v>56</v>
@@ -1283,13 +1297,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" t="s">
         <v>85</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>86</v>
-      </c>
-      <c r="C2" t="s">
-        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Centralised Simulation Configuration Parameters
</commit_message>
<xml_diff>
--- a/resources/configurations/COMPETES EU 2050-KIP config.xlsx
+++ b/resources/configurations/COMPETES EU 2050-KIP config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\workspace\Spine_EMLab_COMPETES\resources\configurations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF236DA9-DCE9-40B9-B67C-2AD0CB2B78A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70188604-A398-4B8B-9061-88AD64ACE48E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="480" windowWidth="38640" windowHeight="21240" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="990" windowWidth="28800" windowHeight="15435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Object Type 1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="93">
   <si>
     <t>Biomass Potential</t>
   </si>
@@ -305,6 +305,12 @@
   </si>
   <si>
     <t>NL Installed Capacity Decentralized (+heat)</t>
+  </si>
+  <si>
+    <t>parameter_index2</t>
+  </si>
+  <si>
+    <t>parameter_index3</t>
   </si>
 </sst>
 </file>
@@ -715,13 +721,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3C637E7-CEF7-493D-BBA4-CB3536D77CE6}">
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -731,8 +737,14 @@
       <c r="C1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -743,7 +755,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -754,7 +766,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -765,7 +777,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -776,7 +788,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -787,7 +799,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -798,7 +810,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -809,7 +821,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -820,7 +832,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>34</v>
       </c>
@@ -831,7 +843,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -842,7 +854,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -856,7 +868,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -867,7 +879,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>37</v>
       </c>
@@ -878,7 +890,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>38</v>
       </c>
@@ -889,7 +901,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>39</v>
       </c>
@@ -1164,8 +1176,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D1116B6-FED4-4FC1-A1F7-3491680046AC}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>